<commit_message>
Update acronym-key and version files
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF6B8C6-CEE5-467A-B561-CF99B19B4B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3D3BC4-E38C-4CE7-B620-30F1E00DB810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="24090" windowHeight="14700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
     <sheet name="Key to Variables" sheetId="1" r:id="rId2"/>
     <sheet name="Key to Top Level Folders" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -328,9 +328,6 @@
     <t>FoVObE</t>
   </si>
   <si>
-    <t>PCiCDTdtTDM</t>
-  </si>
-  <si>
     <t>PTFURfE</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
     <t>Fraction of Vehicles Owned by Entity</t>
   </si>
   <si>
-    <t>Perc Change in Cargo Dist Transported due to TDM</t>
-  </si>
-  <si>
     <t>Percentage Transportation Fuel Use Reduction for Electricity</t>
   </si>
   <si>
@@ -1910,6 +1904,12 @@
   </si>
   <si>
     <t>Share of Building Retrofit Costs Borne by Government</t>
+  </si>
+  <si>
+    <t>RTMF</t>
+  </si>
+  <si>
+    <t>Recipient Transportation Mode Fractions</t>
   </si>
 </sst>
 </file>
@@ -2471,319 +2471,319 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B57" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2827,13 +2827,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2841,15 +2841,15 @@
         <v>4</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
       <c r="F2" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G2" s="32"/>
     </row>
@@ -2864,7 +2864,7 @@
         <v>8</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2872,15 +2872,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G4" s="19"/>
     </row>
@@ -2895,7 +2895,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>24</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2917,16 +2917,16 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2940,10 +2940,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2951,16 +2951,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>463</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>465</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>466</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>467</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2974,7 +2974,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2982,16 +2982,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2999,13 +2999,13 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3019,7 +3019,7 @@
         <v>27</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3033,7 +3033,7 @@
         <v>28</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>29</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3055,13 +3055,13 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
         <v>30</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3083,13 +3083,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3103,10 +3103,10 @@
         <v>31</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>32</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3134,10 +3134,10 @@
         <v>33</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3151,7 +3151,7 @@
         <v>34</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3165,7 +3165,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3173,16 +3173,16 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>436</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3190,16 +3190,16 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3207,13 +3207,13 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3221,13 +3221,13 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3235,15 +3235,15 @@
         <v>9</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="27"/>
       <c r="F28" s="30" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G28" s="27"/>
     </row>
@@ -3252,15 +3252,15 @@
         <v>9</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C29" s="27" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
       <c r="F29" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G29" s="27"/>
     </row>
@@ -3269,17 +3269,17 @@
         <v>9</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27" t="s">
         <v>11</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G30" s="27"/>
     </row>
@@ -3288,17 +3288,17 @@
         <v>9</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G31" s="19"/>
     </row>
@@ -3307,15 +3307,15 @@
         <v>36</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
       <c r="F32" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G32" s="27"/>
     </row>
@@ -3327,13 +3327,13 @@
         <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>38</v>
       </c>
       <c r="F33" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3341,23 +3341,23 @@
         <v>36</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>500</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>501</v>
+      </c>
+      <c r="D34" s="19" t="s">
         <v>502</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>503</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>504</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G34" s="19"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="27" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>5</v>
@@ -3368,206 +3368,206 @@
       <c r="D35" s="27"/>
       <c r="E35" s="27"/>
       <c r="F35" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G35" s="27"/>
     </row>
     <row r="36" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
       <c r="F36" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>536</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="27" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D42" s="27"/>
       <c r="E42" s="27"/>
       <c r="F42" s="36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
+        <v>505</v>
+      </c>
+      <c r="B43" s="27" t="s">
         <v>507</v>
       </c>
-      <c r="B43" s="27" t="s">
-        <v>509</v>
-      </c>
       <c r="C43" s="27" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
       <c r="F43" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G43" s="27"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
       <c r="F44" s="38" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="G44" s="27"/>
       <c r="H44" s="27"/>
     </row>
     <row r="45" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="27" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E45" s="19"/>
       <c r="F45" s="36" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="33" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B46" s="33" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C46" s="33" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G46" s="33" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -3581,7 +3581,7 @@
         <v>42</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3589,13 +3589,13 @@
         <v>39</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
         <v>43</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="29" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3617,18 +3617,18 @@
         <v>39</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D50" s="24"/>
       <c r="E50" s="24"/>
       <c r="F50" s="23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G50" s="24" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3636,13 +3636,13 @@
         <v>44</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3650,13 +3650,13 @@
         <v>44</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3664,13 +3664,13 @@
         <v>44</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3684,10 +3684,10 @@
         <v>57</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3695,13 +3695,13 @@
         <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3709,13 +3709,13 @@
         <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>58</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3737,16 +3737,16 @@
         <v>44</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3754,13 +3754,13 @@
         <v>44</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3768,16 +3768,16 @@
         <v>44</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="F60" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
         <v>59</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3805,10 +3805,10 @@
         <v>60</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3816,13 +3816,13 @@
         <v>44</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3830,13 +3830,13 @@
         <v>44</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3850,7 +3850,7 @@
         <v>61</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -3864,10 +3864,10 @@
         <v>62</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3875,13 +3875,13 @@
         <v>44</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -3895,10 +3895,10 @@
         <v>63</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3909,14 +3909,14 @@
         <v>52</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3924,17 +3924,17 @@
         <v>44</v>
       </c>
       <c r="B70" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D70" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>362</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3942,16 +3942,16 @@
         <v>44</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3959,16 +3959,16 @@
         <v>44</v>
       </c>
       <c r="B72" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>570</v>
-      </c>
       <c r="F72" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -3976,16 +3976,16 @@
         <v>44</v>
       </c>
       <c r="B73" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G73" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>378</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3993,13 +3993,13 @@
         <v>44</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4007,13 +4007,13 @@
         <v>44</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -4027,10 +4027,10 @@
         <v>64</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4038,13 +4038,13 @@
         <v>44</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4052,13 +4052,13 @@
         <v>44</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4066,16 +4066,16 @@
         <v>44</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="D79" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>601</v>
-      </c>
       <c r="F79" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4083,16 +4083,16 @@
         <v>44</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4100,13 +4100,13 @@
         <v>44</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>65</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4128,13 +4128,13 @@
         <v>44</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4142,13 +4142,13 @@
         <v>44</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4156,13 +4156,13 @@
         <v>44</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4176,10 +4176,10 @@
         <v>66</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4187,13 +4187,13 @@
         <v>44</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4201,13 +4201,13 @@
         <v>44</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4215,16 +4215,16 @@
         <v>44</v>
       </c>
       <c r="B89" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="F89" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4232,16 +4232,16 @@
         <v>44</v>
       </c>
       <c r="B90" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="D90" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>556</v>
-      </c>
       <c r="F90" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4249,16 +4249,16 @@
         <v>44</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4266,13 +4266,13 @@
         <v>44</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4286,7 +4286,7 @@
         <v>67</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4294,148 +4294,148 @@
         <v>44</v>
       </c>
       <c r="B94" s="19" t="s">
+        <v>427</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="D94" s="19" t="s">
         <v>429</v>
-      </c>
-      <c r="C94" s="19" t="s">
-        <v>430</v>
-      </c>
-      <c r="D94" s="19" t="s">
-        <v>431</v>
       </c>
       <c r="E94" s="19"/>
       <c r="F94" s="23" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G94" s="19" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B99" s="2" t="s">
-        <v>345</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="19" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C103" s="19" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D103" s="19"/>
       <c r="E103" s="19"/>
       <c r="F103" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G103" s="19"/>
     </row>
@@ -4444,15 +4444,15 @@
         <v>68</v>
       </c>
       <c r="B104" s="27" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C104" s="27" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D104" s="27"/>
       <c r="E104" s="27"/>
       <c r="F104" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G104" s="27"/>
     </row>
@@ -4461,16 +4461,16 @@
         <v>68</v>
       </c>
       <c r="B105" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C105" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>584</v>
-      </c>
       <c r="F105" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4478,16 +4478,16 @@
         <v>68</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="D106" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="C106" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>464</v>
-      </c>
       <c r="F106" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4501,10 +4501,10 @@
         <v>72</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F107" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4512,13 +4512,13 @@
         <v>68</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4532,10 +4532,10 @@
         <v>73</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4543,13 +4543,13 @@
         <v>68</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F110" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4557,16 +4557,16 @@
         <v>68</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F111" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4574,16 +4574,16 @@
         <v>68</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F112" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4591,16 +4591,16 @@
         <v>68</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F113" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -4617,7 +4617,7 @@
         <v>75</v>
       </c>
       <c r="F114" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -4625,17 +4625,17 @@
         <v>68</v>
       </c>
       <c r="B115" s="27" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D115" s="27" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E115" s="27"/>
       <c r="F115" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G115" s="27"/>
     </row>
@@ -4644,15 +4644,15 @@
         <v>68</v>
       </c>
       <c r="B116" s="27" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C116" s="27" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D116" s="27"/>
       <c r="E116" s="27"/>
       <c r="F116" s="37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G116" s="27"/>
     </row>
@@ -4661,160 +4661,160 @@
         <v>68</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F117" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="B118" s="33" t="s">
         <v>494</v>
       </c>
-      <c r="B118" s="33" t="s">
+      <c r="C118" s="33" t="s">
+        <v>495</v>
+      </c>
+      <c r="D118" s="33" t="s">
         <v>496</v>
-      </c>
-      <c r="C118" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="D118" s="33" t="s">
-        <v>498</v>
       </c>
       <c r="E118" s="33"/>
       <c r="F118" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G118" s="33"/>
     </row>
     <row r="119" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="B119" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="B119" s="13" t="s">
-        <v>441</v>
-      </c>
       <c r="C119" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F119" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="122" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D122" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="124" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C124" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="125" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="29" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B125" s="29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C125" s="29" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D125" s="29"/>
       <c r="E125" s="29"/>
       <c r="F125" s="36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G125" s="29" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="126" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="24" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B126" s="24" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C126" s="24" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D126" s="24"/>
       <c r="E126" s="24"/>
       <c r="F126" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G126" s="24"/>
     </row>
@@ -4823,13 +4823,13 @@
         <v>76</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F127" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4837,15 +4837,15 @@
         <v>76</v>
       </c>
       <c r="B128" s="27" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C128" s="27" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D128" s="27"/>
       <c r="E128" s="27"/>
       <c r="F128" s="37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G128" s="27"/>
     </row>
@@ -4860,11 +4860,11 @@
         <v>82</v>
       </c>
       <c r="D129" s="27" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E129" s="27"/>
       <c r="F129" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G129" s="27"/>
     </row>
@@ -4873,16 +4873,16 @@
         <v>76</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4890,13 +4890,13 @@
         <v>76</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4904,13 +4904,13 @@
         <v>76</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="133" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4924,7 +4924,7 @@
         <v>83</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -4932,13 +4932,13 @@
         <v>76</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F134" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4952,10 +4952,10 @@
         <v>84</v>
       </c>
       <c r="F135" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4963,15 +4963,15 @@
         <v>76</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D136" s="13"/>
       <c r="E136" s="13"/>
       <c r="F136" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4979,13 +4979,13 @@
         <v>76</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4999,10 +4999,10 @@
         <v>85</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F138" s="30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5010,13 +5010,13 @@
         <v>76</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5024,13 +5024,13 @@
         <v>76</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F140" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5038,13 +5038,13 @@
         <v>76</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F141" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5052,13 +5052,13 @@
         <v>76</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="143" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -5072,10 +5072,10 @@
         <v>86</v>
       </c>
       <c r="F143" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G143" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="144" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5083,15 +5083,15 @@
         <v>76</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D144" s="27"/>
       <c r="E144" s="27"/>
       <c r="F144" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G144" s="27"/>
     </row>
@@ -5100,15 +5100,15 @@
         <v>76</v>
       </c>
       <c r="B145" s="27" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D145" s="27"/>
       <c r="E145" s="27"/>
       <c r="F145" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G145" s="27"/>
     </row>
@@ -5117,182 +5117,182 @@
         <v>76</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D146" s="19"/>
       <c r="E146" s="19"/>
       <c r="F146" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G146" s="19"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B147" s="27" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D147" s="27"/>
       <c r="E147" s="27"/>
       <c r="F147" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G147" s="27"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B148" s="27" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D148" s="27"/>
       <c r="E148" s="27"/>
       <c r="F148" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G148" s="27"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C149" s="32" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D149" s="32"/>
       <c r="E149" s="32"/>
       <c r="F149" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G149" s="32"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B150" s="27" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D150" s="27"/>
       <c r="E150" s="27"/>
       <c r="F150" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G150" s="27"/>
     </row>
     <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A151" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B151" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="C151" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="D151" s="27" t="s">
         <v>565</v>
-      </c>
-      <c r="C151" s="27" t="s">
-        <v>566</v>
-      </c>
-      <c r="D151" s="27" t="s">
-        <v>567</v>
       </c>
       <c r="E151" s="27"/>
       <c r="F151" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G151" s="27"/>
     </row>
     <row r="152" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B152" s="27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C152" s="27" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F152" s="37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B153" s="32" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C153" s="32" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D153" s="32"/>
       <c r="E153" s="32"/>
       <c r="F153" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G153" s="32"/>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="27" t="s">
+        <v>516</v>
+      </c>
+      <c r="B154" s="27" t="s">
         <v>518</v>
       </c>
-      <c r="B154" s="27" t="s">
+      <c r="C154" s="27" t="s">
         <v>520</v>
-      </c>
-      <c r="C154" s="27" t="s">
-        <v>522</v>
       </c>
       <c r="D154" s="27"/>
       <c r="E154" s="27"/>
       <c r="F154" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G154" s="27"/>
     </row>
     <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D155" s="27"/>
       <c r="E155" s="27"/>
       <c r="F155" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G155" s="27"/>
     </row>
     <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B156" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="C156" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="D156" s="27" t="s">
         <v>590</v>
-      </c>
-      <c r="C156" s="27" t="s">
-        <v>591</v>
-      </c>
-      <c r="D156" s="27" t="s">
-        <v>592</v>
       </c>
       <c r="E156" s="27"/>
       <c r="F156" s="4"/>
@@ -5300,274 +5300,274 @@
     </row>
     <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B157" s="27" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C157" s="27" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D157" s="27"/>
       <c r="E157" s="27" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F157" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G157" s="27"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B158" s="27" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="C158" s="27" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D158" s="27"/>
       <c r="E158" s="27"/>
       <c r="F158" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G158" s="27"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B159" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="C159" s="27" t="s">
         <v>521</v>
-      </c>
-      <c r="C159" s="27" t="s">
-        <v>523</v>
       </c>
       <c r="D159" s="27"/>
       <c r="E159" s="27"/>
       <c r="F159" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G159" s="27"/>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="D160" s="27"/>
       <c r="E160" s="27"/>
       <c r="F160" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G160" s="27"/>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27"/>
       <c r="F161" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G161" s="27"/>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27"/>
       <c r="F162" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G162" s="27"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="27" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27"/>
       <c r="F163" s="35" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G163" s="27"/>
     </row>
     <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="19" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B164" s="19" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C164" s="19" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D164" s="19"/>
       <c r="E164" s="19"/>
       <c r="F164" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G164" s="19"/>
     </row>
     <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F165" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E166" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>114</v>
-      </c>
       <c r="F166" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F167" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F168" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="F169" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F170" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F171" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B173" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="B173" s="19" t="s">
-        <v>114</v>
-      </c>
       <c r="C173" s="19" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D173" s="19"/>
       <c r="E173" s="19"/>
       <c r="F173" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G173" s="19"/>
     </row>
@@ -5582,10 +5582,10 @@
         <v>89</v>
       </c>
       <c r="F174" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G174" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -5593,16 +5593,16 @@
         <v>87</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C175" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C175" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="F175" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5610,18 +5610,18 @@
         <v>87</v>
       </c>
       <c r="B176" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C176" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="C176" s="19" t="s">
-        <v>244</v>
       </c>
       <c r="D176" s="19"/>
       <c r="E176" s="19"/>
       <c r="F176" s="25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G176" s="19" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5632,10 +5632,10 @@
         <v>91</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F177" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5646,10 +5646,10 @@
         <v>92</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F178" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5657,13 +5657,13 @@
         <v>90</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F179" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5671,13 +5671,13 @@
         <v>90</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F180" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5685,13 +5685,13 @@
         <v>90</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F181" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5699,13 +5699,13 @@
         <v>90</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F182" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5713,16 +5713,16 @@
         <v>90</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F183" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
@@ -5730,13 +5730,13 @@
         <v>90</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F184" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5744,13 +5744,13 @@
         <v>90</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F185" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -5758,13 +5758,13 @@
         <v>90</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="F186" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5772,13 +5772,13 @@
         <v>90</v>
       </c>
       <c r="B187" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F187" s="6" t="s">
         <v>298</v>
-      </c>
-      <c r="C187" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F187" s="6" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
@@ -5786,13 +5786,13 @@
         <v>90</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5800,13 +5800,13 @@
         <v>90</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F189" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
@@ -5814,13 +5814,13 @@
         <v>90</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5828,16 +5828,16 @@
         <v>90</v>
       </c>
       <c r="B191" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C191" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="F191" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="C191" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="F191" s="7" t="s">
-        <v>359</v>
-      </c>
       <c r="G191" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -5845,13 +5845,13 @@
         <v>90</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -5862,10 +5862,10 @@
         <v>93</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F193" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -5876,10 +5876,10 @@
         <v>94</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F194" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
@@ -5890,10 +5890,10 @@
         <v>95</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F195" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -5904,10 +5904,10 @@
         <v>96</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -5915,13 +5915,13 @@
         <v>90</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F197" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -5929,13 +5929,13 @@
         <v>90</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F198" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -5946,10 +5946,10 @@
         <v>97</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F199" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5957,16 +5957,16 @@
         <v>90</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F200" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G200" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5974,16 +5974,16 @@
         <v>90</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F201" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5991,16 +5991,16 @@
         <v>90</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F202" s="18" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -6008,16 +6008,16 @@
         <v>90</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F203" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6025,19 +6025,19 @@
         <v>90</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F204" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>90</v>
       </c>
@@ -6045,41 +6045,41 @@
         <v>98</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F205" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="F205" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>99</v>
+        <v>543</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F206" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>544</v>
+      </c>
+      <c r="F206" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G206" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>545</v>
+        <v>624</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="F207" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G207" s="2" t="s">
-        <v>459</v>
+        <v>625</v>
+      </c>
+      <c r="F207" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6087,16 +6087,16 @@
         <v>90</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E208" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F208" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6104,13 +6104,13 @@
         <v>90</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F209" s="16" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6118,13 +6118,13 @@
         <v>90</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F210" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="211" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -6132,13 +6132,13 @@
         <v>90</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F211" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -6146,13 +6146,13 @@
         <v>90</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="F212" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6160,13 +6160,13 @@
         <v>90</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F213" s="14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6174,13 +6174,13 @@
         <v>90</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F214" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="215" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6188,99 +6188,99 @@
         <v>90</v>
       </c>
       <c r="B215" s="19" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C215" s="19" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D215" s="19"/>
       <c r="E215" s="19"/>
       <c r="F215" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G215" s="19"/>
     </row>
     <row r="216" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C216" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D216" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F216" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F217" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B218" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D218" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="C218" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="F218" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F219" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B220" s="19" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C220" s="19" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D220" s="19" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E220" s="19"/>
       <c r="F220" s="20" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G220" s="19"/>
     </row>
@@ -6310,7 +6310,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6318,7 +6318,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6326,7 +6326,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -6334,31 +6334,31 @@
         <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="B6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="B7" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6366,7 +6366,7 @@
         <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -6374,15 +6374,15 @@
         <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6390,23 +6390,23 @@
         <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6414,23 +6414,23 @@
         <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B15" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -6438,7 +6438,7 @@
         <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -6446,15 +6446,15 @@
         <v>90</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to include new 3.1 output graph and current acronym key
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3D3BC4-E38C-4CE7-B620-30F1E00DB810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B462A0-B870-41FB-918E-D0D38D0DFC78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="915" windowWidth="24555" windowHeight="17085" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="629">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -1258,9 +1258,6 @@
     <t>You wish to use 20-year GWP values instead of 100-year GWP values for GHGs (other than F-gases)</t>
   </si>
   <si>
-    <t>You wish to include the emissions associated with the generation of imported electricity (which occur outside the modeled region) in the modeled region's emissions outputs</t>
-  </si>
-  <si>
     <t>You want carbon pricing to only apply to energy-related emissions, exempting non-energy emissions associated with industrial, agricultural, and waste management operations</t>
   </si>
   <si>
@@ -1910,6 +1907,18 @@
   </si>
   <si>
     <t>Recipient Transportation Mode Fractions</t>
+  </si>
+  <si>
+    <t>BIEfEE</t>
+  </si>
+  <si>
+    <t>Boolean Include Emissions from Exported Electricity</t>
+  </si>
+  <si>
+    <t>You wish to include the emissions associated with the generation of exported electricity (which occur inside the modeled region) from the modeled region's emissions outputs.  (The default is enabled.)</t>
+  </si>
+  <si>
+    <t>You wish to include the emissions associated with the generation of imported electricity (which occur outside the modeled region) in the modeled region's emissions outputs  (The default is disabled.)</t>
   </si>
 </sst>
 </file>
@@ -2794,7 +2803,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H220"/>
+  <dimension ref="A1:H221"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2827,7 +2836,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>115</v>
@@ -2841,10 +2850,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>561</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>562</v>
       </c>
       <c r="D2" s="32"/>
       <c r="E2" s="32"/>
@@ -2951,13 +2960,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>462</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>463</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>464</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>465</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>118</v>
@@ -2988,7 +2997,7 @@
         <v>195</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>117</v>
@@ -3083,10 +3092,10 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>591</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>592</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>118</v>
@@ -3173,16 +3182,16 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>434</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>435</v>
       </c>
       <c r="F24" s="18" t="s">
         <v>376</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3190,10 +3199,10 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>376</v>
@@ -3207,10 +3216,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>556</v>
       </c>
       <c r="F26" s="5" t="s">
         <v>117</v>
@@ -3221,10 +3230,10 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>623</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>118</v>
@@ -3252,10 +3261,10 @@
         <v>9</v>
       </c>
       <c r="B29" s="27" t="s">
+        <v>594</v>
+      </c>
+      <c r="C29" s="27" t="s">
         <v>595</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>596</v>
       </c>
       <c r="D29" s="27"/>
       <c r="E29" s="27"/>
@@ -3269,10 +3278,10 @@
         <v>9</v>
       </c>
       <c r="B30" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="C30" s="27" t="s">
         <v>559</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>560</v>
       </c>
       <c r="D30" s="27"/>
       <c r="E30" s="27" t="s">
@@ -3288,10 +3297,10 @@
         <v>9</v>
       </c>
       <c r="B31" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>557</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>558</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19" t="s">
@@ -3307,10 +3316,10 @@
         <v>36</v>
       </c>
       <c r="B32" s="27" t="s">
+        <v>497</v>
+      </c>
+      <c r="C32" s="27" t="s">
         <v>498</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>499</v>
       </c>
       <c r="D32" s="27"/>
       <c r="E32" s="27"/>
@@ -3327,7 +3336,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>38</v>
@@ -3341,13 +3350,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="19" t="s">
+        <v>499</v>
+      </c>
+      <c r="C34" s="19" t="s">
         <v>500</v>
       </c>
-      <c r="C34" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>501</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>502</v>
       </c>
       <c r="E34" s="19"/>
       <c r="F34" s="20" t="s">
@@ -3377,10 +3386,10 @@
         <v>206</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>539</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>540</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19"/>
@@ -3393,7 +3402,7 @@
     </row>
     <row r="37" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>398</v>
@@ -3410,41 +3419,41 @@
     </row>
     <row r="38" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>535</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>418</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>419</v>
       </c>
       <c r="F39" s="7" t="s">
         <v>214</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>315</v>
@@ -3456,132 +3465,135 @@
         <v>214</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>330</v>
+        <v>625</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>331</v>
+        <v>626</v>
       </c>
       <c r="F41" s="7" t="s">
         <v>214</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="B42" s="27" t="s">
-        <v>212</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="36" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="G42" s="27" t="s">
-        <v>407</v>
+      <c r="G42" s="2" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>507</v>
+        <v>212</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>510</v>
+        <v>213</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="27"/>
-      <c r="F43" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F43" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="27" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>509</v>
       </c>
       <c r="D44" s="27"/>
       <c r="E44" s="27"/>
-      <c r="F44" s="38" t="s">
+      <c r="F44" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G44" s="27"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>507</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>508</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-    </row>
-    <row r="45" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="B45" s="19" t="s">
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+    </row>
+    <row r="46" spans="1:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="27" t="s">
+        <v>504</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="C46" s="19" t="s">
         <v>571</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="D46" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="E46" s="19"/>
+      <c r="F46" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="G46" s="19" t="s">
         <v>572</v>
       </c>
-      <c r="D45" s="19" t="s">
-        <v>583</v>
-      </c>
-      <c r="E45" s="19"/>
-      <c r="F45" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
-        <v>593</v>
-      </c>
-      <c r="B46" s="33" t="s">
+    </row>
+    <row r="47" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="33" t="s">
+        <v>592</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>544</v>
+      </c>
+      <c r="C47" s="33" t="s">
         <v>545</v>
       </c>
-      <c r="C46" s="33" t="s">
-        <v>546</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="34" t="s">
+      <c r="D47" s="33"/>
+      <c r="E47" s="33"/>
+      <c r="F47" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="G46" s="33" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>116</v>
+      <c r="G47" s="33" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -3589,60 +3601,60 @@
         <v>39</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>248</v>
+        <v>40</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>249</v>
+        <v>42</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="27" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="27" t="s">
+      <c r="B49" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C50" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="28" t="s">
+      <c r="F50" s="28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="50" spans="1:7" s="29" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
+    <row r="51" spans="1:7" s="29" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="24" t="s">
+      <c r="B51" s="24" t="s">
+        <v>466</v>
+      </c>
+      <c r="C51" s="24" t="s">
         <v>467</v>
       </c>
-      <c r="C50" s="24" t="s">
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="G51" s="24" t="s">
         <v>468</v>
-      </c>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="23" t="s">
-        <v>376</v>
-      </c>
-      <c r="G50" s="24" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F51" s="16" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3650,13 +3662,13 @@
         <v>44</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>117</v>
+        <v>180</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3664,44 +3676,44 @@
         <v>44</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>402</v>
+        <v>216</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>45</v>
+        <v>402</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>228</v>
+        <v>45</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>117</v>
+        <v>57</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3709,13 +3721,13 @@
         <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>118</v>
+        <v>229</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3723,106 +3735,106 @@
         <v>44</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>209</v>
+        <v>46</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>271</v>
+        <v>202</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>47</v>
+        <v>271</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>59</v>
+        <v>270</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>233</v>
+        <v>48</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>116</v>
+        <v>60</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3830,10 +3842,10 @@
         <v>44</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>177</v>
+        <v>233</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>178</v>
+        <v>234</v>
       </c>
       <c r="F64" s="4" t="s">
         <v>116</v>
@@ -3844,79 +3856,75 @@
         <v>44</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>49</v>
+        <v>177</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="F65" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>382</v>
+        <v>50</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>51</v>
+        <v>382</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>383</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="4" t="s">
-        <v>116</v>
+        <v>63</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3924,17 +3932,17 @@
         <v>44</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>358</v>
+        <v>52</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>359</v>
+        <v>200</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>360</v>
+        <v>201</v>
       </c>
       <c r="E70" s="3"/>
-      <c r="F70" s="5" t="s">
-        <v>117</v>
+      <c r="F70" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3942,16 +3950,17 @@
         <v>44</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>116</v>
+        <v>358</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3959,47 +3968,50 @@
         <v>44</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>566</v>
+        <v>198</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>567</v>
+        <v>199</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>568</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>546</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>482</v>
+        <v>565</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="F73" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>566</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>512</v>
+        <v>481</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>118</v>
+        <v>482</v>
+      </c>
+      <c r="F74" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4007,44 +4019,44 @@
         <v>44</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>511</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>53</v>
+        <v>333</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>367</v>
+        <v>334</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>370</v>
+        <v>53</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>371</v>
+        <v>64</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>367</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4052,61 +4064,61 @@
         <v>44</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>485</v>
+        <v>370</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>486</v>
+        <v>371</v>
       </c>
       <c r="F78" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>597</v>
+        <v>484</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>598</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>485</v>
+      </c>
+      <c r="F79" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>211</v>
+        <v>596</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>597</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F81" s="14" t="s">
-        <v>314</v>
+        <v>210</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4114,13 +4126,13 @@
         <v>44</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>54</v>
+        <v>181</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>116</v>
+        <v>182</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4128,13 +4140,13 @@
         <v>44</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>243</v>
+        <v>54</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>117</v>
+        <v>65</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4142,10 +4154,10 @@
         <v>44</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>204</v>
+        <v>243</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>117</v>
@@ -4156,44 +4168,44 @@
         <v>44</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="F85" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>55</v>
+        <v>183</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>223</v>
+        <v>55</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>116</v>
+        <v>66</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4201,64 +4213,61 @@
         <v>44</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>250</v>
+        <v>221</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>552</v>
+        <v>250</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>553</v>
+        <v>251</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>226</v>
+        <v>551</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>227</v>
+        <v>552</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>314</v>
+        <v>553</v>
+      </c>
+      <c r="F91" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4266,13 +4275,16 @@
         <v>44</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>116</v>
+        <v>227</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4280,48 +4292,48 @@
         <v>44</v>
       </c>
       <c r="B93" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F93" s="6" t="s">
+      <c r="F94" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="19" t="s">
+    <row r="95" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B94" s="19" t="s">
+      <c r="B95" s="19" t="s">
+        <v>426</v>
+      </c>
+      <c r="C95" s="19" t="s">
         <v>427</v>
       </c>
-      <c r="C94" s="19" t="s">
+      <c r="D95" s="19" t="s">
         <v>428</v>
       </c>
-      <c r="D94" s="19" t="s">
+      <c r="E95" s="19"/>
+      <c r="F95" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="G95" s="19" t="s">
         <v>429</v>
-      </c>
-      <c r="E94" s="19"/>
-      <c r="F94" s="23" t="s">
-        <v>376</v>
-      </c>
-      <c r="G94" s="19" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4329,10 +4341,10 @@
         <v>341</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>117</v>
@@ -4343,10 +4355,10 @@
         <v>341</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>117</v>
@@ -4357,10 +4369,10 @@
         <v>341</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>117</v>
@@ -4371,202 +4383,199 @@
         <v>341</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>341</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>514</v>
+        <v>343</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+      <c r="F100" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>341</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>218</v>
+        <v>513</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>341</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="19" t="s">
+    <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="B103" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F103" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="B104" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="C104" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="22" t="s">
+      <c r="D104" s="19"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G103" s="19"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B104" s="27" t="s">
-        <v>578</v>
-      </c>
-      <c r="C104" s="27" t="s">
-        <v>579</v>
-      </c>
-      <c r="D104" s="27"/>
-      <c r="E104" s="27"/>
-      <c r="F104" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="19"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B105" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>582</v>
-      </c>
+      <c r="B105" s="27" t="s">
+        <v>577</v>
+      </c>
+      <c r="C105" s="27" t="s">
+        <v>578</v>
+      </c>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
       <c r="F105" s="4" t="s">
         <v>116</v>
       </c>
+      <c r="G105" s="27"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>460</v>
+        <v>579</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>461</v>
+        <v>580</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>462</v>
+        <v>581</v>
       </c>
       <c r="F106" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>69</v>
+        <v>459</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>72</v>
+        <v>460</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>332</v>
+        <v>461</v>
       </c>
       <c r="F107" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>386</v>
+        <v>69</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="F108" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>70</v>
+        <v>386</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F109" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>384</v>
+        <v>70</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>473</v>
+        <v>384</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="F111" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G111" s="2" t="s">
-        <v>479</v>
+        <v>385</v>
+      </c>
+      <c r="F111" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4574,16 +4583,16 @@
         <v>68</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F112" s="18" t="s">
         <v>376</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4591,161 +4600,161 @@
         <v>68</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F113" s="18" t="s">
         <v>376</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="F114" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C114" s="2" t="s">
+      <c r="C115" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="D115" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F114" s="4" t="s">
+      <c r="F115" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="B115" s="27" t="s">
-        <v>456</v>
-      </c>
-      <c r="C115" s="27" t="s">
-        <v>416</v>
-      </c>
-      <c r="D115" s="27" t="s">
-        <v>417</v>
-      </c>
-      <c r="E115" s="27"/>
-      <c r="F115" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="G115" s="27"/>
-    </row>
-    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A116" s="27" t="s">
         <v>68</v>
       </c>
       <c r="B116" s="27" t="s">
+        <v>455</v>
+      </c>
+      <c r="C116" s="27" t="s">
+        <v>415</v>
+      </c>
+      <c r="D116" s="27" t="s">
+        <v>416</v>
+      </c>
+      <c r="E116" s="27"/>
+      <c r="F116" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G116" s="27"/>
+    </row>
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A117" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B117" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="C117" s="27" t="s">
         <v>471</v>
       </c>
-      <c r="C116" s="27" t="s">
-        <v>472</v>
-      </c>
-      <c r="D116" s="27"/>
-      <c r="E116" s="27"/>
-      <c r="F116" s="37" t="s">
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="G116" s="27"/>
-    </row>
-    <row r="117" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+      <c r="G117" s="27"/>
+    </row>
+    <row r="118" spans="1:7" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B118" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="C118" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="C117" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="F117" s="25" t="s">
+      <c r="F118" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G117" s="2" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="33" t="s">
-        <v>492</v>
-      </c>
-      <c r="B118" s="33" t="s">
+      <c r="G118" s="2" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="33" t="s">
+        <v>491</v>
+      </c>
+      <c r="B119" s="33" t="s">
+        <v>493</v>
+      </c>
+      <c r="C119" s="33" t="s">
         <v>494</v>
       </c>
-      <c r="C118" s="33" t="s">
+      <c r="D119" s="33" t="s">
         <v>495</v>
       </c>
-      <c r="D118" s="33" t="s">
-        <v>496</v>
-      </c>
-      <c r="E118" s="33"/>
-      <c r="F118" s="21" t="s">
+      <c r="E119" s="33"/>
+      <c r="F119" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G118" s="33"/>
-    </row>
-    <row r="119" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="13" t="s">
-        <v>437</v>
-      </c>
-      <c r="B119" s="13" t="s">
-        <v>439</v>
-      </c>
-      <c r="C119" s="13" t="s">
-        <v>446</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>118</v>
-      </c>
+      <c r="G119" s="33"/>
     </row>
     <row r="120" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C120" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="F120" s="5" t="s">
-        <v>117</v>
+        <v>445</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C121" s="13" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F121" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="122" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C122" s="13" t="s">
-        <v>449</v>
-      </c>
-      <c r="D122" s="13" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>117</v>
@@ -4753,150 +4762,153 @@
     </row>
     <row r="123" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C123" s="13" t="s">
-        <v>450</v>
+        <v>448</v>
+      </c>
+      <c r="D123" s="13" t="s">
+        <v>452</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="124" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B124" s="13" t="s">
+        <v>442</v>
+      </c>
+      <c r="C124" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="13" t="s">
+        <v>436</v>
+      </c>
+      <c r="B125" s="13" t="s">
+        <v>443</v>
+      </c>
+      <c r="C125" s="13" t="s">
+        <v>450</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G125" s="13" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="B126" s="29" t="s">
         <v>444</v>
       </c>
-      <c r="C124" s="13" t="s">
+      <c r="C126" s="29" t="s">
         <v>451</v>
       </c>
-      <c r="F124" s="7" t="s">
+      <c r="D126" s="29"/>
+      <c r="E126" s="29"/>
+      <c r="F126" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="G124" s="13" t="s">
+      <c r="G126" s="29" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="125" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="29" t="s">
-        <v>437</v>
-      </c>
-      <c r="B125" s="29" t="s">
-        <v>445</v>
-      </c>
-      <c r="C125" s="29" t="s">
-        <v>452</v>
-      </c>
-      <c r="D125" s="29"/>
-      <c r="E125" s="29"/>
-      <c r="F125" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="G125" s="29" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="24" t="s">
-        <v>437</v>
-      </c>
-      <c r="B126" s="24" t="s">
+    <row r="127" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="B127" s="24" t="s">
+        <v>611</v>
+      </c>
+      <c r="C127" s="24" t="s">
         <v>612</v>
       </c>
-      <c r="C126" s="24" t="s">
-        <v>613</v>
-      </c>
-      <c r="D126" s="24"/>
-      <c r="E126" s="24"/>
-      <c r="F126" s="22" t="s">
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G126" s="24"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
+      <c r="G127" s="24"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B128" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="C127" s="2" t="s">
+      <c r="C128" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F127" s="14" t="s">
+      <c r="F128" s="14" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B128" s="27" t="s">
-        <v>604</v>
-      </c>
-      <c r="C128" s="27" t="s">
-        <v>605</v>
-      </c>
-      <c r="D128" s="27"/>
-      <c r="E128" s="27"/>
-      <c r="F128" s="37" t="s">
-        <v>116</v>
-      </c>
-      <c r="G128" s="27"/>
-    </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="27" t="s">
         <v>76</v>
       </c>
       <c r="B129" s="27" t="s">
+        <v>603</v>
+      </c>
+      <c r="C129" s="27" t="s">
+        <v>604</v>
+      </c>
+      <c r="D129" s="27"/>
+      <c r="E129" s="27"/>
+      <c r="F129" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="G129" s="27"/>
+    </row>
+    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B130" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C129" s="27" t="s">
+      <c r="C130" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D129" s="27" t="s">
-        <v>466</v>
-      </c>
-      <c r="E129" s="27"/>
-      <c r="F129" s="30" t="s">
-        <v>488</v>
-      </c>
-      <c r="G129" s="27"/>
-    </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F130" s="31" t="s">
-        <v>376</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>415</v>
-      </c>
+      <c r="D130" s="27" t="s">
+        <v>465</v>
+      </c>
+      <c r="E130" s="27"/>
+      <c r="F130" s="30" t="s">
+        <v>487</v>
+      </c>
+      <c r="G130" s="27"/>
     </row>
     <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>400</v>
+        <v>244</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>118</v>
+        <v>245</v>
+      </c>
+      <c r="F131" s="31" t="s">
+        <v>376</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4904,10 +4916,10 @@
         <v>76</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>616</v>
+        <v>400</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>617</v>
+        <v>401</v>
       </c>
       <c r="F132" s="6" t="s">
         <v>118</v>
@@ -4918,27 +4930,27 @@
         <v>76</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>78</v>
+        <v>615</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F133" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+        <v>616</v>
+      </c>
+      <c r="F133" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>610</v>
+        <v>78</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="F134" s="6" t="s">
-        <v>118</v>
+        <v>83</v>
+      </c>
+      <c r="F134" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -4946,16 +4958,13 @@
         <v>76</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>79</v>
+        <v>609</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F135" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>425</v>
+        <v>610</v>
+      </c>
+      <c r="F135" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
@@ -4963,15 +4972,16 @@
         <v>76</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>537</v>
+        <v>79</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="D136" s="13"/>
-      <c r="E136" s="13"/>
-      <c r="F136" s="6" t="s">
-        <v>118</v>
+        <v>84</v>
+      </c>
+      <c r="F136" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4979,30 +4989,29 @@
         <v>76</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>246</v>
+        <v>536</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="F137" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>537</v>
+      </c>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>80</v>
+        <v>246</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D138" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="F138" s="30" t="s">
-        <v>488</v>
+        <v>247</v>
+      </c>
+      <c r="F138" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5010,13 +5019,16 @@
         <v>76</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>237</v>
+        <v>80</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F139" s="5" t="s">
-        <v>117</v>
+        <v>85</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="F139" s="30" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5024,13 +5036,13 @@
         <v>76</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>347</v>
+        <v>237</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="F140" s="6" t="s">
-        <v>118</v>
+        <v>238</v>
+      </c>
+      <c r="F140" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5038,10 +5050,10 @@
         <v>76</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F141" s="6" t="s">
         <v>118</v>
@@ -5052,58 +5064,55 @@
         <v>76</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="F142" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+      <c r="F142" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B143" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F143" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B144" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C144" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F143" s="18" t="s">
+      <c r="F144" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="G143" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B144" s="27" t="s">
-        <v>585</v>
-      </c>
-      <c r="C144" s="27" t="s">
-        <v>584</v>
-      </c>
-      <c r="D144" s="27"/>
-      <c r="E144" s="27"/>
-      <c r="F144" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="G144" s="27"/>
+      <c r="G144" s="2" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="145" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="27" t="s">
         <v>76</v>
       </c>
       <c r="B145" s="27" t="s">
-        <v>606</v>
+        <v>584</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>607</v>
+        <v>583</v>
       </c>
       <c r="D145" s="27"/>
       <c r="E145" s="27"/>
@@ -5112,49 +5121,49 @@
       </c>
       <c r="G145" s="27"/>
     </row>
-    <row r="146" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="19" t="s">
+    <row r="146" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B146" s="19" t="s">
+      <c r="B146" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="C146" s="27" t="s">
+        <v>606</v>
+      </c>
+      <c r="D146" s="27"/>
+      <c r="E146" s="27"/>
+      <c r="F146" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="G146" s="27"/>
+    </row>
+    <row r="147" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>607</v>
+      </c>
+      <c r="C147" s="19" t="s">
         <v>608</v>
       </c>
-      <c r="C146" s="19" t="s">
-        <v>609</v>
-      </c>
-      <c r="D146" s="19"/>
-      <c r="E146" s="19"/>
-      <c r="F146" s="22" t="s">
+      <c r="D147" s="19"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G146" s="19"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B147" s="27" t="s">
-        <v>526</v>
-      </c>
-      <c r="C147" s="27" t="s">
-        <v>527</v>
-      </c>
-      <c r="D147" s="27"/>
-      <c r="E147" s="27"/>
-      <c r="F147" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G147" s="27"/>
+      <c r="G147" s="19"/>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B148" s="27" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D148" s="27"/>
       <c r="E148" s="27"/>
@@ -5165,114 +5174,114 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B149" s="32" t="s">
-        <v>489</v>
-      </c>
-      <c r="C149" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="D149" s="32"/>
-      <c r="E149" s="32"/>
+        <v>515</v>
+      </c>
+      <c r="B149" s="27" t="s">
+        <v>527</v>
+      </c>
+      <c r="C149" s="27" t="s">
+        <v>528</v>
+      </c>
+      <c r="D149" s="27"/>
+      <c r="E149" s="27"/>
       <c r="F149" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G149" s="32"/>
+      <c r="G149" s="27"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B150" s="27" t="s">
-        <v>530</v>
-      </c>
-      <c r="C150" s="27" t="s">
-        <v>531</v>
-      </c>
-      <c r="D150" s="27"/>
-      <c r="E150" s="27"/>
+        <v>515</v>
+      </c>
+      <c r="B150" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="C150" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="D150" s="32"/>
+      <c r="E150" s="32"/>
       <c r="F150" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="G150" s="27"/>
-    </row>
-    <row r="151" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G150" s="32"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B151" s="27" t="s">
-        <v>563</v>
+        <v>529</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>564</v>
-      </c>
-      <c r="D151" s="27" t="s">
-        <v>565</v>
-      </c>
+        <v>530</v>
+      </c>
+      <c r="D151" s="27"/>
       <c r="E151" s="27"/>
       <c r="F151" s="4" t="s">
         <v>116</v>
       </c>
       <c r="G151" s="27"/>
     </row>
-    <row r="152" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A152" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B152" s="27" t="s">
+        <v>562</v>
+      </c>
+      <c r="C152" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="D152" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="E152" s="27"/>
+      <c r="F152" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G152" s="27"/>
+    </row>
+    <row r="153" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="B153" s="27" t="s">
+        <v>531</v>
+      </c>
+      <c r="C153" s="27" t="s">
         <v>532</v>
       </c>
-      <c r="C152" s="27" t="s">
-        <v>533</v>
-      </c>
-      <c r="F152" s="37" t="s">
+      <c r="F153" s="37" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A153" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B153" s="32" t="s">
+    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A154" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="B154" s="32" t="s">
+        <v>523</v>
+      </c>
+      <c r="C154" s="32" t="s">
         <v>524</v>
       </c>
-      <c r="C153" s="32" t="s">
-        <v>525</v>
-      </c>
-      <c r="D153" s="32"/>
-      <c r="E153" s="32"/>
-      <c r="F153" s="6" t="s">
+      <c r="D154" s="32"/>
+      <c r="E154" s="32"/>
+      <c r="F154" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="G153" s="32"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B154" s="27" t="s">
-        <v>518</v>
-      </c>
-      <c r="C154" s="27" t="s">
-        <v>520</v>
-      </c>
-      <c r="D154" s="27"/>
-      <c r="E154" s="27"/>
-      <c r="F154" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G154" s="27"/>
-    </row>
-    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G154" s="32"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B155" s="27" t="s">
-        <v>602</v>
+        <v>517</v>
       </c>
       <c r="C155" s="27" t="s">
-        <v>603</v>
+        <v>519</v>
       </c>
       <c r="D155" s="27"/>
       <c r="E155" s="27"/>
@@ -5283,66 +5292,66 @@
     </row>
     <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B156" s="27" t="s">
-        <v>588</v>
+        <v>601</v>
       </c>
       <c r="C156" s="27" t="s">
-        <v>589</v>
-      </c>
-      <c r="D156" s="27" t="s">
-        <v>590</v>
-      </c>
+        <v>602</v>
+      </c>
+      <c r="D156" s="27"/>
       <c r="E156" s="27"/>
-      <c r="F156" s="4"/>
+      <c r="F156" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="G156" s="27"/>
     </row>
     <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B157" s="27" t="s">
+        <v>587</v>
+      </c>
+      <c r="C157" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="D157" s="27" t="s">
+        <v>589</v>
+      </c>
+      <c r="E157" s="27"/>
+      <c r="F157" s="4"/>
+      <c r="G157" s="27"/>
+    </row>
+    <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="B158" s="27" t="s">
+        <v>617</v>
+      </c>
+      <c r="C158" s="27" t="s">
         <v>618</v>
       </c>
-      <c r="C157" s="27" t="s">
-        <v>619</v>
-      </c>
-      <c r="D157" s="27"/>
-      <c r="E157" s="27" t="s">
-        <v>518</v>
-      </c>
-      <c r="F157" s="4" t="s">
+      <c r="D158" s="27"/>
+      <c r="E158" s="27" t="s">
+        <v>517</v>
+      </c>
+      <c r="F158" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="G157" s="27"/>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="27" t="s">
-        <v>516</v>
-      </c>
-      <c r="B158" s="27" t="s">
-        <v>614</v>
-      </c>
-      <c r="C158" s="27" t="s">
-        <v>615</v>
-      </c>
-      <c r="D158" s="27"/>
-      <c r="E158" s="27"/>
-      <c r="F158" s="6" t="s">
-        <v>118</v>
       </c>
       <c r="G158" s="27"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B159" s="27" t="s">
-        <v>519</v>
+        <v>613</v>
       </c>
       <c r="C159" s="27" t="s">
-        <v>521</v>
+        <v>614</v>
       </c>
       <c r="D159" s="27"/>
       <c r="E159" s="27"/>
@@ -5353,13 +5362,13 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B160" s="27" t="s">
-        <v>574</v>
+        <v>518</v>
       </c>
       <c r="C160" s="27" t="s">
-        <v>575</v>
+        <v>520</v>
       </c>
       <c r="D160" s="27"/>
       <c r="E160" s="27"/>
@@ -5370,13 +5379,13 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B161" s="27" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C161" s="27" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="D161" s="27"/>
       <c r="E161" s="27"/>
@@ -5387,98 +5396,101 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B162" s="27" t="s">
-        <v>620</v>
+        <v>575</v>
       </c>
       <c r="C162" s="27" t="s">
-        <v>621</v>
+        <v>576</v>
       </c>
       <c r="D162" s="27"/>
       <c r="E162" s="27"/>
-      <c r="F162" s="4" t="s">
-        <v>116</v>
+      <c r="F162" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="G162" s="27"/>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="27" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B163" s="27" t="s">
-        <v>522</v>
+        <v>619</v>
       </c>
       <c r="C163" s="27" t="s">
-        <v>523</v>
+        <v>620</v>
       </c>
       <c r="D163" s="27"/>
       <c r="E163" s="27"/>
-      <c r="F163" s="35" t="s">
+      <c r="F163" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="G163" s="27"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="27" t="s">
+        <v>515</v>
+      </c>
+      <c r="B164" s="27" t="s">
+        <v>521</v>
+      </c>
+      <c r="C164" s="27" t="s">
+        <v>522</v>
+      </c>
+      <c r="D164" s="27"/>
+      <c r="E164" s="27"/>
+      <c r="F164" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="G163" s="27"/>
-    </row>
-    <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="19" t="s">
-        <v>516</v>
-      </c>
-      <c r="B164" s="19" t="s">
+      <c r="G164" s="27"/>
+    </row>
+    <row r="165" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A165" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="B165" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="C165" s="19" t="s">
         <v>600</v>
       </c>
-      <c r="C164" s="19" t="s">
-        <v>601</v>
-      </c>
-      <c r="D164" s="19"/>
-      <c r="E164" s="19"/>
-      <c r="F164" s="21" t="s">
+      <c r="D165" s="19"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="G164" s="19"/>
-    </row>
-    <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F165" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G165" s="19"/>
+    </row>
+    <row r="166" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>377</v>
+        <v>256</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E166" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F166" s="14" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>258</v>
+        <v>377</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F167" s="6" t="s">
-        <v>118</v>
+        <v>378</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F167" s="14" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5486,16 +5498,13 @@
         <v>110</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="F168" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G168" s="2" t="s">
-        <v>426</v>
+        <v>259</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5503,41 +5512,44 @@
         <v>110</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="F169" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="F169" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G169" s="2" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>111</v>
+        <v>262</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>114</v>
+        <v>267</v>
       </c>
       <c r="F170" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>263</v>
+        <v>111</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F171" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
+      </c>
+      <c r="F171" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -5545,97 +5557,97 @@
         <v>110</v>
       </c>
       <c r="B172" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F172" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B173" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C172" s="2" t="s">
+      <c r="C173" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="F172" s="14" t="s">
+      <c r="F173" s="14" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="173" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="19" t="s">
+    <row r="174" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A174" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="B173" s="19" t="s">
+      <c r="B174" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C173" s="19" t="s">
+      <c r="C174" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="D173" s="19"/>
-      <c r="E173" s="19"/>
-      <c r="F173" s="22" t="s">
+      <c r="D174" s="19"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G173" s="19"/>
-    </row>
-    <row r="174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A174" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F174" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G174" s="2" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G174" s="19"/>
+    </row>
+    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B175" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G175" s="2" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B176" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C176" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="F175" s="7" t="s">
+      <c r="F176" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G175" s="2" t="s">
+      <c r="G176" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="176" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="19" t="s">
+    <row r="177" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A177" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B176" s="19" t="s">
+      <c r="B177" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C176" s="19" t="s">
+      <c r="C177" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="D176" s="19"/>
-      <c r="E176" s="19"/>
-      <c r="F176" s="25" t="s">
+      <c r="D177" s="19"/>
+      <c r="E177" s="19"/>
+      <c r="F177" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G176" s="19" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A177" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B177" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F177" s="5" t="s">
-        <v>117</v>
+      <c r="G177" s="19" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5643,13 +5655,13 @@
         <v>90</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F178" s="6" t="s">
-        <v>118</v>
+        <v>99</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
@@ -5657,13 +5669,13 @@
         <v>90</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>503</v>
+        <v>92</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="F179" s="5" t="s">
-        <v>117</v>
+        <v>100</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
@@ -5671,72 +5683,72 @@
         <v>90</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>353</v>
+        <v>502</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="F180" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>503</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>320</v>
+        <v>353</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>321</v>
+        <v>354</v>
       </c>
       <c r="F181" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>278</v>
+        <v>320</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>279</v>
+        <v>321</v>
       </c>
       <c r="F182" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="E183" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="F183" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="F183" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F184" s="4" t="s">
-        <v>116</v>
+        <v>293</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="F184" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
@@ -5744,10 +5756,10 @@
         <v>90</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F185" s="4" t="s">
         <v>116</v>
@@ -5758,41 +5770,41 @@
         <v>90</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="F186" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="F186" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="F187" s="6" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="F188" s="6" t="s">
-        <v>118</v>
+        <v>298</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
@@ -5800,10 +5812,10 @@
         <v>90</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>423</v>
+        <v>284</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>424</v>
+        <v>285</v>
       </c>
       <c r="F189" s="6" t="s">
         <v>118</v>
@@ -5814,44 +5826,44 @@
         <v>90</v>
       </c>
       <c r="B190" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B191" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C190" s="2" t="s">
+      <c r="C191" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="F190" s="5" t="s">
+      <c r="F191" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="191" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A191" s="13" t="s">
+    <row r="192" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A192" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B191" s="13" t="s">
+      <c r="B192" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="C191" s="13" t="s">
+      <c r="C192" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="F191" s="7" t="s">
+      <c r="F192" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="G191" s="2" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A192" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B192" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="F192" s="5" t="s">
-        <v>117</v>
+      <c r="G192" s="2" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
@@ -5859,13 +5871,13 @@
         <v>90</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>93</v>
+        <v>420</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F193" s="6" t="s">
-        <v>118</v>
+        <v>421</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
@@ -5873,10 +5885,10 @@
         <v>90</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F194" s="6" t="s">
         <v>118</v>
@@ -5887,10 +5899,10 @@
         <v>90</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F195" s="6" t="s">
         <v>118</v>
@@ -5901,13 +5913,13 @@
         <v>90</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F196" s="5" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+      <c r="F196" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -5915,10 +5927,10 @@
         <v>90</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>548</v>
+        <v>96</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>549</v>
+        <v>104</v>
       </c>
       <c r="F197" s="5" t="s">
         <v>117</v>
@@ -5929,10 +5941,10 @@
         <v>90</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>586</v>
+        <v>547</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>587</v>
+        <v>548</v>
       </c>
       <c r="F198" s="5" t="s">
         <v>117</v>
@@ -5943,30 +5955,27 @@
         <v>90</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>97</v>
+        <v>585</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F199" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="200" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>586</v>
+      </c>
+      <c r="F199" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>363</v>
+        <v>97</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="F200" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G200" s="2" t="s">
-        <v>411</v>
+        <v>105</v>
+      </c>
+      <c r="F200" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="201" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5974,16 +5983,16 @@
         <v>90</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F201" s="18" t="s">
         <v>376</v>
       </c>
       <c r="G201" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="202" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -5991,33 +6000,33 @@
         <v>90</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>301</v>
+        <v>365</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>302</v>
+        <v>366</v>
       </c>
       <c r="F202" s="18" t="s">
         <v>376</v>
       </c>
       <c r="G202" s="2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="F203" s="6" t="s">
-        <v>118</v>
+        <v>302</v>
+      </c>
+      <c r="F203" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G203" s="2" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -6025,61 +6034,64 @@
         <v>90</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F204" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="205" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="F204" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>98</v>
+        <v>286</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>106</v>
+        <v>287</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>284</v>
       </c>
       <c r="F205" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="206" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>543</v>
+        <v>98</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="F206" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G206" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="F206" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>624</v>
+        <v>542</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>625</v>
-      </c>
-      <c r="F207" s="6" t="s">
-        <v>118</v>
+        <v>543</v>
+      </c>
+      <c r="F207" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="G207" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
@@ -6087,16 +6099,13 @@
         <v>90</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>299</v>
+        <v>623</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="F208" s="5" t="s">
-        <v>117</v>
+        <v>624</v>
+      </c>
+      <c r="F208" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -6104,13 +6113,16 @@
         <v>90</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="F209" s="16" t="s">
-        <v>322</v>
+        <v>300</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F209" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -6118,41 +6130,41 @@
         <v>90</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>369</v>
+        <v>309</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="F210" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="F210" s="16" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>305</v>
+        <v>369</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="F211" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+      <c r="F211" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F212" s="6" t="s">
-        <v>118</v>
+        <v>306</v>
+      </c>
+      <c r="F212" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -6160,13 +6172,13 @@
         <v>90</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="F213" s="14" t="s">
-        <v>314</v>
+        <v>291</v>
+      </c>
+      <c r="F213" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -6174,115 +6186,129 @@
         <v>90</v>
       </c>
       <c r="B214" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="F214" s="14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B215" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C214" s="2" t="s">
+      <c r="C215" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="F214" s="6" t="s">
+      <c r="F215" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="19" t="s">
+    <row r="216" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A216" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="B215" s="19" t="s">
+      <c r="B216" s="19" t="s">
         <v>379</v>
       </c>
-      <c r="C215" s="19" t="s">
+      <c r="C216" s="19" t="s">
         <v>380</v>
       </c>
-      <c r="D215" s="19"/>
-      <c r="E215" s="19"/>
-      <c r="F215" s="22" t="s">
+      <c r="D216" s="19"/>
+      <c r="E216" s="19"/>
+      <c r="F216" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="G215" s="19"/>
-    </row>
-    <row r="216" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A216" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B216" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C216" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="F216" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G216" s="19"/>
+    </row>
+    <row r="217" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>269</v>
+        <v>108</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>268</v>
+        <v>109</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>491</v>
+        <v>388</v>
       </c>
       <c r="F217" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>311</v>
+        <v>269</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>312</v>
+        <v>268</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>313</v>
+        <v>490</v>
       </c>
       <c r="F218" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B219" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D219" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="F219" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C220" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="C219" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="F219" s="5" t="s">
+      <c r="F220" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="19" t="s">
+    <row r="221" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A221" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="B220" s="19" t="s">
+      <c r="B221" s="19" t="s">
         <v>361</v>
       </c>
-      <c r="C220" s="19" t="s">
+      <c r="C221" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="D220" s="19" t="s">
+      <c r="D221" s="19" t="s">
         <v>381</v>
       </c>
-      <c r="E220" s="19"/>
-      <c r="F220" s="20" t="s">
+      <c r="E221" s="19"/>
+      <c r="F221" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="G220" s="19"/>
+      <c r="G221" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6347,18 +6373,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B6" t="s">
         <v>505</v>
-      </c>
-      <c r="B6" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>592</v>
+      </c>
+      <c r="B7" t="s">
         <v>593</v>
-      </c>
-      <c r="B7" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -6395,18 +6421,18 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>491</v>
+      </c>
+      <c r="B12" t="s">
         <v>492</v>
-      </c>
-      <c r="B12" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>436</v>
+      </c>
+      <c r="B13" t="s">
         <v>437</v>
-      </c>
-      <c r="B13" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6419,10 +6445,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>515</v>
+      </c>
+      <c r="B15" t="s">
         <v>516</v>
-      </c>
-      <c r="B15" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>